<commit_message>
added the updated lecture plan
</commit_message>
<xml_diff>
--- a/Vorlesungsplan.xlsx
+++ b/Vorlesungsplan.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Wissensrepräsentation – Knowledge Graphs</t>
   </si>
   <si>
-    <t xml:space="preserve">Überwachtes ML – Lineare Regression</t>
+    <t xml:space="preserve">Einführung – Python-Implementierung von Graphen-Suchroblemen</t>
   </si>
   <si>
     <t xml:space="preserve">Teamaufgabe</t>
@@ -71,6 +71,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -92,12 +93,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,20 +145,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,127 +292,127 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="62.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.06"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>45772</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>45779</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>45786</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>45793</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>45800</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="3" t="n">
         <v>45807</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+      <c r="A9" s="3" t="n">
         <v>45814</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="0" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="A10" s="3" t="n">
         <v>45821</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+      <c r="A11" s="3" t="n">
         <v>45828</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>45835</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>